<commit_message>
Update the excel file Wei Sili position statistics.
</commit_message>
<xml_diff>
--- a/卫斯理仓位统计.xlsx
+++ b/卫斯理仓位统计.xlsx
@@ -74,7 +74,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="181" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -115,14 +115,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -647,244 +650,291 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C1" sqref="C1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>499</v>
-      </c>
-      <c r="C1">
+        <v>699</v>
+      </c>
+      <c r="C1" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D1">
         <v>0</v>
       </c>
-      <c r="D1">
-        <f>C1*B1</f>
+      <c r="E1">
+        <f>D1*B1</f>
         <v>0</v>
       </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>210</v>
-      </c>
-      <c r="C2">
+        <v>312</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D2">
         <v>5</v>
       </c>
-      <c r="D2">
-        <f>C2*B2</f>
-        <v>1050</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <f>D2*B2</f>
+        <v>1560</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B3">
-        <v>286</v>
-      </c>
-      <c r="C3">
+        <v>428</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D3">
         <v>15</v>
       </c>
-      <c r="D3">
-        <f>C3*B3</f>
-        <v>4290</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f>D3*B3</f>
+        <v>6420</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>342</v>
-      </c>
-      <c r="C4">
+        <v>495</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D4">
         <v>25</v>
       </c>
-      <c r="D4">
-        <f>C4*B4</f>
-        <v>8550</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f>D4*B4</f>
+        <v>12375</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>320</v>
-      </c>
-      <c r="C5">
+        <v>464</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D5">
         <v>35</v>
       </c>
-      <c r="D5">
-        <f>C5*B5</f>
-        <v>11200</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f>D5*B5</f>
+        <v>16240</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>411</v>
-      </c>
-      <c r="C6">
+        <v>584</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D6">
         <v>45</v>
       </c>
-      <c r="D6">
-        <f>C6*B6</f>
-        <v>18495</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f>D6*B6</f>
+        <v>26280</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>565</v>
-      </c>
-      <c r="C7">
+        <v>848</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D7">
         <v>55</v>
       </c>
-      <c r="D7">
-        <f>C7*B7</f>
-        <v>31075</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f>D7*B7</f>
+        <v>46640</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>528</v>
-      </c>
-      <c r="C8">
+        <v>760</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D8">
         <v>65</v>
       </c>
-      <c r="D8">
-        <f>C8*B8</f>
-        <v>34320</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f>D8*B8</f>
+        <v>49400</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>627</v>
-      </c>
-      <c r="C9">
+        <v>897</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D9">
         <v>75</v>
       </c>
-      <c r="D9">
-        <f>C9*B9</f>
-        <v>47025</v>
-      </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f>D9*B9</f>
+        <v>67275</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>816</v>
-      </c>
-      <c r="C10">
+        <v>1163</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D10">
         <v>85</v>
       </c>
-      <c r="D10">
-        <f>C10*B10</f>
-        <v>69360</v>
-      </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f>D10*B10</f>
+        <v>98855</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1207</v>
-      </c>
-      <c r="C11">
+        <v>1670</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="D11">
         <v>95</v>
       </c>
-      <c r="D11">
-        <f>C11*B11</f>
-        <v>114665</v>
-      </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f>D11*B11</f>
+        <v>158650</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1278</v>
-      </c>
-      <c r="C12">
+        <v>1770</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="D12">
         <v>100</v>
       </c>
-      <c r="D12">
-        <f>C12*B12</f>
-        <v>127800</v>
-      </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f>D12*B12</f>
+        <v>177000</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>572</v>
-      </c>
-      <c r="C13">
+        <v>786</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D13">
         <v>100</v>
       </c>
-      <c r="D13">
-        <f>C13*B13</f>
-        <v>57200</v>
-      </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f>D13*B13</f>
+        <v>78600</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>1480</v>
-      </c>
-      <c r="E14" s="2">
-        <f>SUM(D1:D13)/SUM(B1:B13)</f>
-        <v>68.532828612452676</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2224</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="F14" s="2">
+        <f>SUM(E1:E13)/SUM(B1:B13)</f>
+        <v>67.974898859874955</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15">
         <f>SUM(B1:B14)</f>
-        <v>9141</v>
+        <v>13100</v>
+      </c>
+      <c r="C15">
+        <f>SUM(C1:C14)</f>
+        <v>0.92</v>
       </c>
       <c r="E15" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Try low volatility features in script.
</commit_message>
<xml_diff>
--- a/卫斯理仓位统计.xlsx
+++ b/卫斯理仓位统计.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9744" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9744" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="20191010" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,8 @@
     <sheet name="20191015" sheetId="3" r:id="rId3"/>
     <sheet name="20191017" sheetId="4" r:id="rId4"/>
     <sheet name="20191021" sheetId="5" r:id="rId5"/>
+    <sheet name="20191023" sheetId="6" r:id="rId6"/>
+    <sheet name="20191027" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="22">
   <si>
     <t>空仓</t>
   </si>
@@ -79,6 +81,21 @@
   </si>
   <si>
     <t>空仓 (已选)</t>
+  </si>
+  <si>
+    <t>看多</t>
+  </si>
+  <si>
+    <t>看空 (已选)</t>
+  </si>
+  <si>
+    <t>看平</t>
+  </si>
+  <si>
+    <t>看空</t>
+  </si>
+  <si>
+    <t>看平 (已选)</t>
   </si>
 </sst>
 </file>
@@ -423,10 +440,13 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -956,7 +976,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1234,13 +1254,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1502,6 +1525,60 @@
         <v>0.93</v>
       </c>
       <c r="E15" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>4544</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>3367</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>1541</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>2063</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f>SUM(B20:B23)</f>
+        <v>11515</v>
+      </c>
+      <c r="C24" s="3">
+        <f>SUM(C20:C23)</f>
+        <v>0.98</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1515,17 +1592,20 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C14"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B1">
-        <v>444</v>
+        <v>837</v>
       </c>
       <c r="C1" s="3">
         <v>7.0000000000000007E-2</v>
@@ -1543,17 +1623,17 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>173</v>
+        <v>349</v>
       </c>
       <c r="C2" s="3">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="E2">
         <f t="shared" si="0"/>
-        <v>865</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1561,7 +1641,7 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>206</v>
+        <v>401</v>
       </c>
       <c r="C3" s="3">
         <v>0.03</v>
@@ -1571,7 +1651,7 @@
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>3090</v>
+        <v>6015</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1579,7 +1659,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>221</v>
+        <v>460</v>
       </c>
       <c r="C4" s="3">
         <v>0.03</v>
@@ -1589,7 +1669,7 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>5525</v>
+        <v>11500</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1597,7 +1677,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>235</v>
+        <v>475</v>
       </c>
       <c r="C5" s="3">
         <v>0.04</v>
@@ -1607,7 +1687,7 @@
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>8225</v>
+        <v>16625</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1615,7 +1695,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>240</v>
+        <v>487</v>
       </c>
       <c r="C6" s="3">
         <v>0.04</v>
@@ -1625,7 +1705,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>10800</v>
+        <v>21915</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1633,17 +1713,17 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>369</v>
+        <v>671</v>
       </c>
       <c r="C7" s="3">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="D7">
         <v>55</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>20295</v>
+        <v>36905</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1651,7 +1731,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>294</v>
+        <v>584</v>
       </c>
       <c r="C8" s="3">
         <v>0.05</v>
@@ -1661,7 +1741,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>19110</v>
+        <v>37960</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1669,17 +1749,17 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>347</v>
+        <v>703</v>
       </c>
       <c r="C9" s="3">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="D9">
         <v>75</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>26025</v>
+        <v>52725</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1687,7 +1767,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>432</v>
+        <v>850</v>
       </c>
       <c r="C10" s="3">
         <v>7.0000000000000007E-2</v>
@@ -1697,7 +1777,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>36720</v>
+        <v>72250</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1705,7 +1785,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>702</v>
+        <v>1397</v>
       </c>
       <c r="C11" s="3">
         <v>0.12</v>
@@ -1715,7 +1795,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>66690</v>
+        <v>132715</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1723,17 +1803,17 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>741</v>
+        <v>1363</v>
       </c>
       <c r="C12" s="3">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="D12">
         <v>100</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>74100</v>
+        <v>136300</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1741,17 +1821,17 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>473</v>
+        <v>880</v>
       </c>
       <c r="C13" s="3">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D13">
         <v>100</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>47300</v>
+        <v>88000</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1759,27 +1839,697 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>973</v>
+        <v>2056</v>
       </c>
       <c r="C14" s="3">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="F14" s="2">
         <f>SUM(E1:E13)/SUM(B1:B13)</f>
-        <v>65.356776706992008</v>
+        <v>64.994712911071161</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15">
         <f>SUM(B1:B14)</f>
-        <v>5850</v>
+        <v>11513</v>
       </c>
       <c r="C15">
         <f>SUM(C1:C14)</f>
         <v>0.94000000000000006</v>
       </c>
       <c r="E15" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1">
+        <v>986</v>
+      </c>
+      <c r="C1" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <f t="shared" ref="E1:E13" si="0">D1*B1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>422</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>455</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>6825</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>533</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>13325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>528</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D5">
+        <v>35</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>18480</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>600</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D6">
+        <v>45</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>800</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D7">
+        <v>55</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>672</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D8">
+        <v>65</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>43680</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>775</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D9">
+        <v>75</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>58125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>973</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D10">
+        <v>85</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>82705</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>1617</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="D11">
+        <v>95</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>153615</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1537</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>153700</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>1034</v>
+      </c>
+      <c r="C13" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>103400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>2379</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="F14" s="2">
+        <f>SUM(E1:E13)/SUM(B1:B13)</f>
+        <v>64.66931942919868</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15">
+        <f>SUM(B1:B14)</f>
+        <v>13311</v>
+      </c>
+      <c r="C15">
+        <f>SUM(C1:C14)</f>
+        <v>0.94000000000000006</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>3391</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>5632</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>1836</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>2439</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f>SUM(B20:B23)</f>
+        <v>13298</v>
+      </c>
+      <c r="C24" s="3">
+        <f>SUM(C20:C23)</f>
+        <v>0.98</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1">
+        <v>888</v>
+      </c>
+      <c r="C1" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <f t="shared" ref="E1:E13" si="0">D1*B1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>377</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>436</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>6540</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>504</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>12600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>530</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D5">
+        <v>35</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>18550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>564</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D6">
+        <v>45</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>25380</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>821</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D7">
+        <v>55</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>45155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>724</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D8">
+        <v>65</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>47060</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>838</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D9">
+        <v>75</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>62850</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1017</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D10">
+        <v>85</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>86445</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>1641</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="D11">
+        <v>95</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>155895</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1680</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>168000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>871</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>87100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>2298</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="F14" s="2">
+        <f>SUM(E1:E13)/SUM(B1:B13)</f>
+        <v>65.876411716095859</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15">
+        <f>SUM(B1:B14)</f>
+        <v>13189</v>
+      </c>
+      <c r="C15">
+        <f>SUM(C1:C14)</f>
+        <v>0.93</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>8214</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>1589</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1115</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>2270</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f>SUM(B20:B23)</f>
+        <v>13188</v>
+      </c>
+      <c r="C24" s="3">
+        <f>SUM(C20:C23)</f>
+        <v>0.99</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Update Wei Sili position statistics.
</commit_message>
<xml_diff>
--- a/卫斯理仓位统计.xlsx
+++ b/卫斯理仓位统计.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9744" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9744" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="20191010" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="20191021" sheetId="5" r:id="rId5"/>
     <sheet name="20191023" sheetId="6" r:id="rId6"/>
     <sheet name="20191027" sheetId="7" r:id="rId7"/>
+    <sheet name="20191029" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="22">
   <si>
     <t>空仓</t>
   </si>
@@ -2207,7 +2208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -2536,4 +2537,339 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1">
+        <v>877</v>
+      </c>
+      <c r="C1" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <f t="shared" ref="E1:E13" si="0">D1*B1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>382</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>453</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>6795</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>512</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>12800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>567</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D5">
+        <v>35</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>19845</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>599</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D6">
+        <v>45</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>26955</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>892</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D7">
+        <v>55</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>49060</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>774</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D8">
+        <v>65</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>50310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>872</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D9">
+        <v>75</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>65400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1125</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D10">
+        <v>85</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>95625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>1802</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="D11">
+        <v>95</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>171190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1759</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>175900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>1149</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>114900</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>2344</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="F14" s="2">
+        <f>SUM(E1:E13)/SUM(B1:B13)</f>
+        <v>67.218396667516785</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15">
+        <f>SUM(B1:B14)</f>
+        <v>14107</v>
+      </c>
+      <c r="C15">
+        <f>SUM(C1:C14)</f>
+        <v>0.94000000000000006</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>3755</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>6288</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>1761</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>2325</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f>SUM(B20:B23)</f>
+        <v>14129</v>
+      </c>
+      <c r="C24" s="3">
+        <f>SUM(C20:C23)</f>
+        <v>0.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Wei Sili position statistics. Refactor script.
</commit_message>
<xml_diff>
--- a/卫斯理仓位统计.xlsx
+++ b/卫斯理仓位统计.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9744" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9744" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="20191010" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="20191023" sheetId="6" r:id="rId6"/>
     <sheet name="20191027" sheetId="7" r:id="rId7"/>
     <sheet name="20191029" sheetId="8" r:id="rId8"/>
+    <sheet name="20191103" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="24">
   <si>
     <t>空仓</t>
   </si>
@@ -97,6 +98,12 @@
   </si>
   <si>
     <t>看平 (已选)</t>
+  </si>
+  <si>
+    <t>看多 (已选)</t>
+  </si>
+  <si>
+    <t>我是来给卫斯理打Call的~</t>
   </si>
 </sst>
 </file>
@@ -2543,7 +2550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
@@ -2872,4 +2879,339 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1">
+        <v>812</v>
+      </c>
+      <c r="C1" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <f t="shared" ref="E1:E13" si="0">D1*B1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>336</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>388</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>5820</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>449</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>11225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>487</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D5">
+        <v>35</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>17045</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>558</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D6">
+        <v>45</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>25110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>779</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D7">
+        <v>55</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>42845</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>650</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D8">
+        <v>65</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>42250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>753</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D9">
+        <v>75</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>56475</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>999</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D10">
+        <v>85</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>84915</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>1463</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="D11">
+        <v>95</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>138985</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1535</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>153500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>832</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>83200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>2177</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="F14" s="2">
+        <f>SUM(E1:E13)/SUM(B1:B13)</f>
+        <v>66.034259535902805</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15">
+        <f>SUM(B1:B14)</f>
+        <v>12218</v>
+      </c>
+      <c r="C15">
+        <f>SUM(C1:C14)</f>
+        <v>0.92</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>5942</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>2322</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>1728</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>2225</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f>SUM(B20:B23)</f>
+        <v>12217</v>
+      </c>
+      <c r="C24" s="3">
+        <f>SUM(C20:C23)</f>
+        <v>0.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update WSL position statistics.
</commit_message>
<xml_diff>
--- a/卫斯理仓位统计.xlsx
+++ b/卫斯理仓位统计.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9744" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9744" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="20191010" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="20191027" sheetId="7" r:id="rId7"/>
     <sheet name="20191029" sheetId="8" r:id="rId8"/>
     <sheet name="20191103" sheetId="9" r:id="rId9"/>
+    <sheet name="20191110" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="24">
   <si>
     <t>空仓</t>
   </si>
@@ -688,6 +689,341 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1">
+        <v>284</v>
+      </c>
+      <c r="C1" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <f t="shared" ref="E1:E13" si="0">D1*B1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>133</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>665</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>167</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>2505</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>184</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>227</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D5">
+        <v>35</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>7945</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>210</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D6">
+        <v>45</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>9450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>297</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D7">
+        <v>55</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>16335</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>281</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D8">
+        <v>65</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>18265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>280</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D9">
+        <v>75</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>388</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D10">
+        <v>85</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>32980</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>528</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D11">
+        <v>95</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>50160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>545</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>54500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>324</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>32400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>1349</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F14" s="2">
+        <f>SUM(E1:E13)/SUM(B1:B13)</f>
+        <v>65.178014553014549</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15">
+        <f>SUM(B1:B14)</f>
+        <v>5197</v>
+      </c>
+      <c r="C15">
+        <f>SUM(C1:C14)</f>
+        <v>0.94</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>1255</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>1960</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>620</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>1360</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f>SUM(B20:B23)</f>
+        <v>5195</v>
+      </c>
+      <c r="C24" s="3">
+        <f>SUM(C20:C23)</f>
+        <v>0.98</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
@@ -2885,7 +3221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update WSL position statistics. Add and modify comments.
</commit_message>
<xml_diff>
--- a/卫斯理仓位统计.xlsx
+++ b/卫斯理仓位统计.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9744" firstSheet="5" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9744" firstSheet="7" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="20191010" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,8 @@
     <sheet name="20191117" sheetId="12" r:id="rId12"/>
     <sheet name="20191119" sheetId="14" r:id="rId13"/>
     <sheet name="20191121" sheetId="13" r:id="rId14"/>
+    <sheet name="20191125" sheetId="15" r:id="rId15"/>
+    <sheet name="20191126" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="26">
   <si>
     <t>空仓</t>
   </si>
@@ -112,6 +114,9 @@
   </si>
   <si>
     <t>我是来给卫斯理打call的</t>
+  </si>
+  <si>
+    <t>我是来给卫斯理打call的~</t>
   </si>
 </sst>
 </file>
@@ -2041,7 +2046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -2363,6 +2368,676 @@
       <c r="C24" s="3">
         <f>SUM(C20:C23)</f>
         <v>0.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1">
+        <v>841</v>
+      </c>
+      <c r="C1" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <f t="shared" ref="E1:E13" si="0">D1*B1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>358</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>398</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>5970</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>483</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>12075</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>456</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D5">
+        <v>35</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>15960</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>490</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D6">
+        <v>45</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>22050</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>672</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D7">
+        <v>55</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>36960</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>583</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D8">
+        <v>65</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>37895</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>643</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D9">
+        <v>75</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>48225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>913</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D10">
+        <v>85</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>77605</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>1308</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="D11">
+        <v>95</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>124260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1284</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>128400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>938</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>93800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>2146</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="F14" s="2">
+        <f>SUM(E1:E13)/SUM(B1:B13)</f>
+        <v>64.587381231984622</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15">
+        <f>SUM(B1:B14)</f>
+        <v>11513</v>
+      </c>
+      <c r="C15">
+        <f>SUM(C1:C14)</f>
+        <v>0.94</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>3745</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>4144</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>1456</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>2152</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f>SUM(B20:B23)</f>
+        <v>11497</v>
+      </c>
+      <c r="C24" s="3">
+        <f>SUM(C20:C23)</f>
+        <v>0.98</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1">
+        <v>1105</v>
+      </c>
+      <c r="C1" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <f t="shared" ref="E1:E13" si="0">D1*B1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>423</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>421</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>6315</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>526</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>13150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>522</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D5">
+        <v>35</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>18270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>546</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D6">
+        <v>45</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>24570</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>713</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D7">
+        <v>55</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>39215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>607</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D8">
+        <v>65</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>39455</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>730</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D9">
+        <v>75</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>54750</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>924</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D10">
+        <v>85</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>78540</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>1323</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D11">
+        <v>95</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>125685</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1268</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>126800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>995</v>
+      </c>
+      <c r="C13" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>99500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>2355</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="F14" s="2">
+        <f>SUM(E1:E13)/SUM(B1:B13)</f>
+        <v>62.195882411165002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15">
+        <f>SUM(B1:B14)</f>
+        <v>12458</v>
+      </c>
+      <c r="C15">
+        <f>SUM(C1:C14)</f>
+        <v>0.91999999999999993</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>2713</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>5867</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>1488</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>2372</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f>SUM(B20:B23)</f>
+        <v>12440</v>
+      </c>
+      <c r="C24" s="3">
+        <f>SUM(C20:C23)</f>
+        <v>0.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>